<commit_message>
Added plots and regression
</commit_message>
<xml_diff>
--- a/Task2/TODO.xlsx
+++ b/Task2/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Intro_to_ML\Task2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vukas\Documents\GitHub\Intro_to_ML\Task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65BEE44-85EF-4B16-B3D4-850AF39F2417}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC01F8D-F361-46B9-8AEC-4435A3A2BD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="0" windowWidth="20448" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Imputation</t>
   </si>
@@ -88,13 +88,23 @@
   </si>
   <si>
     <t>Feature vector engineering (read up on time series measurements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualization is done
+The only thing left is to decide which measurements to discard </t>
+  </si>
+  <si>
+    <t>Started, has to be improved</t>
+  </si>
+  <si>
+    <t>global median for now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +135,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -370,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -460,6 +483,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -742,24 +771,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="69.88671875" customWidth="1"/>
+    <col min="2" max="2" width="69.90625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="5" max="5" width="60.88671875" customWidth="1"/>
+    <col min="5" max="5" width="60.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,23 +802,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="25"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="39"/>
+      <c r="E5" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="26"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D6" s="41"/>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
         <v>10</v>
       </c>
@@ -799,15 +832,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="42"/>
+      <c r="E8" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="22" t="s">
         <v>17</v>
       </c>
@@ -815,7 +850,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
@@ -823,31 +858,31 @@
       <c r="D10" s="37"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="22"/>
       <c r="C11" s="29"/>
       <c r="D11" s="37"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="21"/>
       <c r="C12" s="28"/>
       <c r="D12" s="37"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
       <c r="D13" s="38"/>
       <c r="E13" s="36"/>
     </row>
-    <row r="14" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="4"/>
       <c r="C14" s="31"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
@@ -861,7 +896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20" t="s">
         <v>4</v>
       </c>
@@ -869,7 +904,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>5</v>
       </c>
@@ -877,7 +912,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="22" t="s">
         <v>6</v>
       </c>
@@ -885,7 +920,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>7</v>
       </c>
@@ -893,7 +928,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="22" t="s">
         <v>8</v>
       </c>
@@ -901,7 +936,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="13"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
         <v>9</v>
       </c>
@@ -909,19 +944,19 @@
       <c r="D21" s="7"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="24"/>
       <c r="C22" s="33"/>
       <c r="D22" s="10"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="23"/>
       <c r="C23" s="30"/>
       <c r="D23" s="9"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented CrossVal for task 3
</commit_message>
<xml_diff>
--- a/Task2/TODO.xlsx
+++ b/Task2/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Intro_to_ML\Task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65BEE44-85EF-4B16-B3D4-850AF39F2417}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE8CB45-AD4F-4247-90BC-172516787C70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="0" windowWidth="20448" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1104" yWindow="0" windowWidth="20448" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Imputation</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Feature vector engineering (read up on time series measurements)</t>
+  </si>
+  <si>
+    <t>Started, still a lot of options left to play with</t>
+  </si>
+  <si>
+    <t>Need to change standardization in CrossVal, right now it's wrong implem</t>
+  </si>
+  <si>
+    <t>Maybe use feature_selection library to extract best features</t>
   </si>
 </sst>
 </file>
@@ -126,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +166,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -370,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -460,6 +475,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -743,7 +759,7 @@
   <dimension ref="B2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +829,9 @@
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
@@ -882,16 +900,20 @@
         <v>6</v>
       </c>
       <c r="C18" s="27"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="13"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">

</xml_diff>